<commit_message>
added code for error capture and updated imperative changes
</commit_message>
<xml_diff>
--- a/Data/TimecardPunch_Amy2.xlsx
+++ b/Data/TimecardPunch_Amy2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\WFM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4F8CC9-93C7-483E-AF00-8D070E0AC47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6BD072-6815-4C32-BEC1-9AFA01C865CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="45">
   <si>
     <t>EmpNum</t>
   </si>
@@ -52,18 +52,24 @@
     <t>13:00</t>
   </si>
   <si>
+    <t>17:15</t>
+  </si>
+  <si>
+    <t>Failed : You typed an invalid time.</t>
+  </si>
+  <si>
+    <t>Wed 10/02</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>17:15</t>
-  </si>
-  <si>
-    <t>Wed 10/02</t>
-  </si>
-  <si>
     <t>13:30</t>
   </si>
   <si>
+    <t>Passed</t>
+  </si>
+  <si>
     <t>Thu 10/03</t>
   </si>
   <si>
@@ -142,10 +148,7 @@
     <t>14:00</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>No Entries</t>
+    <t>Error -  No Entries or testdata issue</t>
   </si>
   <si>
     <t>14:16</t>
@@ -193,26 +196,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -549,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,14 +575,14 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
+      <c r="E2">
+        <v>0.29992000000000002</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -609,19 +593,19 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -629,22 +613,22 @@
         <v>10649012</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -652,22 +636,22 @@
         <v>10649012</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -675,22 +659,22 @@
         <v>10649012</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -698,22 +682,22 @@
         <v>10649012</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="E7">
-        <v>0.58333333333333337</v>
+      <c r="E7" t="s">
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -721,22 +705,22 @@
         <v>10649012</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -744,22 +728,22 @@
         <v>10649012</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -767,7 +751,7 @@
         <v>10649012</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -776,13 +760,13 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -790,22 +774,22 @@
         <v>10649012</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -813,22 +797,22 @@
         <v>10649012</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -836,22 +820,22 @@
         <v>10649012</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -859,22 +843,22 @@
         <v>10649012</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -882,22 +866,22 @@
         <v>10649012</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -905,22 +889,22 @@
         <v>10649012</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -928,22 +912,22 @@
         <v>10649012</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -951,22 +935,22 @@
         <v>10649012</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -974,22 +958,22 @@
         <v>10649012</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -997,22 +981,22 @@
         <v>10649012</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1020,22 +1004,22 @@
         <v>10649012</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1043,22 +1027,22 @@
         <v>10649012</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1066,22 +1050,22 @@
         <v>10649012</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1089,22 +1073,22 @@
         <v>10649012</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1115,19 +1099,19 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1138,19 +1122,19 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1158,22 +1142,22 @@
         <v>10649023</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1181,22 +1165,22 @@
         <v>10649023</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1204,22 +1188,22 @@
         <v>10649023</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1227,22 +1211,22 @@
         <v>10649023</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1250,22 +1234,22 @@
         <v>10649023</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1273,22 +1257,22 @@
         <v>10649023</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1296,22 +1280,22 @@
         <v>10649023</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1319,22 +1303,22 @@
         <v>10649023</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1342,22 +1326,22 @@
         <v>10649023</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1365,22 +1349,22 @@
         <v>10649023</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F36" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1388,22 +1372,22 @@
         <v>10649023</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1411,22 +1395,22 @@
         <v>10649023</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1434,22 +1418,22 @@
         <v>10649023</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1457,22 +1441,22 @@
         <v>10649023</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1480,22 +1464,22 @@
         <v>10649023</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1503,22 +1487,22 @@
         <v>10649023</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1526,22 +1510,22 @@
         <v>10649023</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D43" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F43" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1549,22 +1533,22 @@
         <v>10649023</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F44" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1572,22 +1556,22 @@
         <v>10649023</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1595,22 +1579,22 @@
         <v>10649023</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F46" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -1618,35 +1602,26 @@
         <v>10649023</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G47" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A1:G47" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
added code for capturing error as well as taking screenshot of that error(WebActionsPage)
</commit_message>
<xml_diff>
--- a/Data/TimecardPunch_Amy2.xlsx
+++ b/Data/TimecardPunch_Amy2.xlsx
@@ -445,7 +445,7 @@
         <v>17:15</v>
       </c>
       <c r="G2" t="str">
-        <v>Failed : You typed an invalid time.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : You typed an invalid time.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-01-50-936Z.png</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         <v>17:15</v>
       </c>
       <c r="G3" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-02-08-853Z.png</v>
       </c>
     </row>
     <row r="4">
@@ -491,7 +491,7 @@
         <v>17:15</v>
       </c>
       <c r="G4" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-02-26-068Z.png</v>
       </c>
     </row>
     <row r="5">
@@ -514,7 +514,7 @@
         <v/>
       </c>
       <c r="G5" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-02-44-429Z.png</v>
       </c>
     </row>
     <row r="6">
@@ -560,7 +560,7 @@
         <v>17:15</v>
       </c>
       <c r="G7" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-03-09-236Z.png</v>
       </c>
     </row>
     <row r="8">
@@ -583,7 +583,7 @@
         <v>17:15</v>
       </c>
       <c r="G8" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-03-27-450Z.png</v>
       </c>
     </row>
     <row r="9">
@@ -606,7 +606,7 @@
         <v>17:15</v>
       </c>
       <c r="G9" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-03-45-634Z.png</v>
       </c>
     </row>
     <row r="10">
@@ -629,7 +629,7 @@
         <v>17:15</v>
       </c>
       <c r="G10" t="str">
-        <v>Passed</v>
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -652,7 +652,7 @@
         <v>17:15</v>
       </c>
       <c r="G11" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-04-39-112Z.png</v>
       </c>
     </row>
     <row r="12">
@@ -675,7 +675,7 @@
         <v>17:15</v>
       </c>
       <c r="G12" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-04-57-164Z.png</v>
       </c>
     </row>
     <row r="13">
@@ -698,7 +698,7 @@
         <v>16:59</v>
       </c>
       <c r="G13" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-05-15-951Z.png</v>
       </c>
     </row>
     <row r="14">
@@ -721,7 +721,7 @@
         <v>17:15</v>
       </c>
       <c r="G14" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-05-34-395Z.png</v>
       </c>
     </row>
     <row r="15">
@@ -744,7 +744,7 @@
         <v>17:15</v>
       </c>
       <c r="G15" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-05-52-673Z.png</v>
       </c>
     </row>
     <row r="16">
@@ -767,7 +767,7 @@
         <v>17:15</v>
       </c>
       <c r="G16" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-06-14-981Z.png</v>
       </c>
     </row>
     <row r="17">
@@ -790,7 +790,7 @@
         <v>17:15</v>
       </c>
       <c r="G17" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v/>
       </c>
     </row>
     <row r="18">
@@ -813,7 +813,7 @@
         <v>17:15</v>
       </c>
       <c r="G18" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v/>
       </c>
     </row>
     <row r="19">
@@ -836,7 +836,7 @@
         <v>17:15</v>
       </c>
       <c r="G19" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v/>
       </c>
     </row>
     <row r="20">
@@ -859,7 +859,7 @@
         <v>17:15</v>
       </c>
       <c r="G20" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v/>
       </c>
     </row>
     <row r="21">
@@ -882,7 +882,7 @@
         <v>17:15</v>
       </c>
       <c r="G21" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v/>
       </c>
     </row>
     <row r="22">
@@ -905,7 +905,7 @@
         <v>17:15</v>
       </c>
       <c r="G22" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v/>
       </c>
     </row>
     <row r="23">
@@ -928,7 +928,7 @@
         <v>17:15</v>
       </c>
       <c r="G23" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v/>
       </c>
     </row>
     <row r="24">
@@ -951,7 +951,7 @@
         <v>17:15</v>
       </c>
       <c r="G24" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v/>
       </c>
     </row>
     <row r="25">
@@ -1020,7 +1020,7 @@
         <v>17:15</v>
       </c>
       <c r="G27" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T10-33-42-879Z.png</v>
       </c>
     </row>
     <row r="28">
@@ -1089,7 +1089,7 @@
         <v/>
       </c>
       <c r="G30" t="str">
-        <v>Failed :  No Entries or testdata issue</v>
+        <v>Failed :  No valid entries or test data issue.</v>
       </c>
     </row>
     <row r="31">
@@ -1158,7 +1158,7 @@
         <v>17:15</v>
       </c>
       <c r="G33" t="str">
-        <v>Failed : [object Promise]find failed screenshot --&gt; [object Promise]</v>
+        <v>Failed : [object Promise]&amp; find failed screenshot --&gt; H:\WFM\WFMFailedScreenShot\2024-11-27T10-34-21-802Z.png</v>
       </c>
     </row>
     <row r="34">
@@ -1250,7 +1250,7 @@
         <v>17:15</v>
       </c>
       <c r="G37" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T10-34-58-837Z.png</v>
       </c>
     </row>
     <row r="38">
@@ -1434,7 +1434,7 @@
         <v>17:15</v>
       </c>
       <c r="G45" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T10-36-01-843Z.png</v>
       </c>
     </row>
     <row r="46">
@@ -1480,7 +1480,7 @@
         <v>17:15</v>
       </c>
       <c r="G47" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;[object Promise]</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T10-36-26-841Z.png</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated code for PunchIn-Out
</commit_message>
<xml_diff>
--- a/Data/TimecardPunch_Amy2.xlsx
+++ b/Data/TimecardPunch_Amy2.xlsx
@@ -445,7 +445,7 @@
         <v>17:15</v>
       </c>
       <c r="G2" t="str">
-        <v>Failed : You typed an invalid time.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-01-50-936Z.png</v>
+        <v>Failed : You typed an invalid time.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-28T08-52-56-234Z.png</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         <v>17:15</v>
       </c>
       <c r="G3" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-02-08-853Z.png</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-28T08-53-06-970Z.png</v>
       </c>
     </row>
     <row r="4">
@@ -491,7 +491,7 @@
         <v>17:15</v>
       </c>
       <c r="G4" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-02-26-068Z.png</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-28T08-53-17-190Z.png</v>
       </c>
     </row>
     <row r="5">
@@ -514,7 +514,7 @@
         <v/>
       </c>
       <c r="G5" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-02-44-429Z.png</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-28T08-53-27-668Z.png</v>
       </c>
     </row>
     <row r="6">
@@ -560,7 +560,7 @@
         <v>17:15</v>
       </c>
       <c r="G7" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-03-09-236Z.png</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-28T08-53-41-439Z.png</v>
       </c>
     </row>
     <row r="8">
@@ -583,7 +583,7 @@
         <v>17:15</v>
       </c>
       <c r="G8" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-03-27-450Z.png</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-28T08-53-51-539Z.png</v>
       </c>
     </row>
     <row r="9">
@@ -606,7 +606,7 @@
         <v>17:15</v>
       </c>
       <c r="G9" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-03-45-634Z.png</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-28T08-54-01-635Z.png</v>
       </c>
     </row>
     <row r="10">
@@ -629,7 +629,7 @@
         <v>17:15</v>
       </c>
       <c r="G10" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="11">
@@ -652,7 +652,7 @@
         <v>17:15</v>
       </c>
       <c r="G11" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-04-39-112Z.png</v>
+        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-28T08-54-44-578Z.png</v>
       </c>
     </row>
     <row r="12">
@@ -675,7 +675,7 @@
         <v>17:15</v>
       </c>
       <c r="G12" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-04-57-164Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="13">
@@ -698,7 +698,7 @@
         <v>16:59</v>
       </c>
       <c r="G13" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-05-15-951Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="14">
@@ -721,7 +721,7 @@
         <v>17:15</v>
       </c>
       <c r="G14" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-05-34-395Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="15">
@@ -744,7 +744,7 @@
         <v>17:15</v>
       </c>
       <c r="G15" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-05-52-673Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="16">
@@ -767,7 +767,7 @@
         <v>17:15</v>
       </c>
       <c r="G16" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T12-06-14-981Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="17">
@@ -790,7 +790,7 @@
         <v>17:15</v>
       </c>
       <c r="G17" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="18">
@@ -813,7 +813,7 @@
         <v>17:15</v>
       </c>
       <c r="G18" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="19">
@@ -836,7 +836,7 @@
         <v>17:15</v>
       </c>
       <c r="G19" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="20">
@@ -859,7 +859,7 @@
         <v>17:15</v>
       </c>
       <c r="G20" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="21">
@@ -882,7 +882,7 @@
         <v>17:15</v>
       </c>
       <c r="G21" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="22">
@@ -905,7 +905,7 @@
         <v>17:15</v>
       </c>
       <c r="G22" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="23">
@@ -928,7 +928,7 @@
         <v>17:15</v>
       </c>
       <c r="G23" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="24">
@@ -951,7 +951,7 @@
         <v>17:15</v>
       </c>
       <c r="G24" t="str">
-        <v/>
+        <v>Passed</v>
       </c>
     </row>
     <row r="25">
@@ -1020,7 +1020,7 @@
         <v>17:15</v>
       </c>
       <c r="G27" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T10-33-42-879Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="28">
@@ -1158,7 +1158,7 @@
         <v>17:15</v>
       </c>
       <c r="G33" t="str">
-        <v>Failed : [object Promise]&amp; find failed screenshot --&gt; H:\WFM\WFMFailedScreenShot\2024-11-27T10-34-21-802Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="34">
@@ -1250,7 +1250,7 @@
         <v>17:15</v>
       </c>
       <c r="G37" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T10-34-58-837Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="38">
@@ -1434,7 +1434,7 @@
         <v>17:15</v>
       </c>
       <c r="G45" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T10-36-01-843Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
     <row r="46">
@@ -1480,7 +1480,7 @@
         <v>17:15</v>
       </c>
       <c r="G47" t="str">
-        <v>Failed : Error Duplicate Punches are not allowed.&amp; find failed Screenshot Path:-&gt;H:\WFM\WFMFailedScreenShot\2024-11-27T10-36-26-841Z.png</v>
+        <v>Passed</v>
       </c>
     </row>
   </sheetData>

</xml_diff>